<commit_message>
Making DDR4 DRAM Symbol and footprint
</commit_message>
<xml_diff>
--- a/docs/DDR4_PinDescription.xlsx
+++ b/docs/DDR4_PinDescription.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\PCB\Project\DDR4_DIMM_Project\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B2CB4CC-593C-4E93-9415-38F547712347}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66899EC3-B385-45A6-9022-5374EF918CC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{5EF2FE71-DCD4-4236-92FA-B5935CC9F8C6}"/>
   </bookViews>
@@ -818,7 +818,7 @@
   <dimension ref="A1:D29"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C33" sqref="C33"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -856,7 +856,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:4" hidden="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A3" s="4" t="s">
         <v>7</v>
       </c>
@@ -870,7 +870,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:4" hidden="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A4" s="4" t="s">
         <v>9</v>
       </c>
@@ -898,7 +898,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:4" hidden="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A6" s="4" t="s">
         <v>13</v>
       </c>
@@ -940,7 +940,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="34.799999999999997" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:4" ht="34.799999999999997" hidden="1" x14ac:dyDescent="0.4">
       <c r="A9" s="7" t="s">
         <v>20</v>
       </c>
@@ -1024,7 +1024,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="1:4" hidden="1" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A15" s="4" t="s">
         <v>32</v>
       </c>
@@ -1038,7 +1038,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:4" hidden="1" x14ac:dyDescent="0.4">
       <c r="A16" s="4" t="s">
         <v>34</v>
       </c>
@@ -1052,7 +1052,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="34.799999999999997" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:4" ht="34.799999999999997" hidden="1" x14ac:dyDescent="0.4">
       <c r="A17" s="7" t="s">
         <v>36</v>
       </c>
@@ -1094,7 +1094,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:4" hidden="1" x14ac:dyDescent="0.4">
       <c r="A20" s="4" t="s">
         <v>43</v>
       </c>
@@ -1108,7 +1108,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="21" spans="1:4" hidden="1" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A21" s="4" t="s">
         <v>44</v>
       </c>
@@ -1238,7 +1238,7 @@
   <autoFilter ref="A1:D29" xr:uid="{B73647BE-74DB-4DA9-91E8-F6F78A1B7639}">
     <filterColumn colId="2">
       <filters>
-        <filter val="Data"/>
+        <filter val="Control"/>
       </filters>
     </filterColumn>
   </autoFilter>

</xml_diff>